<commit_message>
Now compatible for SQL Server 2016
</commit_message>
<xml_diff>
--- a/ExcelTemplates/InstanceInfo.xlsx
+++ b/ExcelTemplates/InstanceInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\GitHub\SQLServerPerformanceTuning\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{043A02C1-DD24-405F-8155-2CB2BE8E267C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE11C16-7796-47BE-82D4-8500823DB302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{10AD8C71-7510-4E2A-9097-D6D1B55202C8}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId12"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="181">
   <si>
     <t>server_name</t>
   </si>
@@ -270,9 +270,6 @@
     <t>softnuma_configuration_desc</t>
   </si>
   <si>
-    <t>process_physical_affinity</t>
-  </si>
-  <si>
     <t>sql_memory_model</t>
   </si>
   <si>
@@ -288,12 +285,6 @@
     <t>numa_node_count</t>
   </si>
   <si>
-    <t>container_type</t>
-  </si>
-  <si>
-    <t>container_type_desc</t>
-  </si>
-  <si>
     <t>memory_clerk_address</t>
   </si>
   <si>
@@ -522,24 +513,6 @@
     <t>page_compression_success_count</t>
   </si>
   <si>
-    <t>version_generated_inrow</t>
-  </si>
-  <si>
-    <t>version_generated_offrow</t>
-  </si>
-  <si>
-    <t>ghost_version_inrow</t>
-  </si>
-  <si>
-    <t>ghost_version_offrow</t>
-  </si>
-  <si>
-    <t>insert_over_ghost_version_inrow</t>
-  </si>
-  <si>
-    <t>insert_over_ghost_version_offrow</t>
-  </si>
-  <si>
     <t>stats_id</t>
   </si>
   <si>
@@ -564,12 +537,6 @@
     <t>is_incremental</t>
   </si>
   <si>
-    <t>has_persisted_sample</t>
-  </si>
-  <si>
-    <t>stats_generation_method_desc</t>
-  </si>
-  <si>
     <t>stats_columns</t>
   </si>
   <si>
@@ -607,12 +574,6 @@
   </si>
   <si>
     <t>average_range_rows</t>
-  </si>
-  <si>
-    <t>object_id2</t>
-  </si>
-  <si>
-    <t>stats_id3</t>
   </si>
   <si>
     <t>(blank)</t>
@@ -669,13 +630,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -711,10 +671,10 @@
       <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+      <numFmt numFmtId="29" formatCode="mm:ss.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="29" formatCode="mm:ss.0"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1043,7 +1003,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE0AA7EF-212B-45A0-B90F-79529C042135}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="schema_object_name">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE0AA7EF-212B-45A0-B90F-79529C042135}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="schema_object_name">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
@@ -1342,9 +1302,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A6B8DD7C-AAB7-4857-88E6-CB63ACE6C9CD}" name="Table4" displayName="Table4" ref="A1:AK2" totalsRowShown="0">
-  <autoFilter ref="A1:AK2" xr:uid="{A6B8DD7C-AAB7-4857-88E6-CB63ACE6C9CD}"/>
-  <tableColumns count="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A6B8DD7C-AAB7-4857-88E6-CB63ACE6C9CD}" name="Table4" displayName="Table4" ref="A1:AH2" totalsRowShown="0">
+  <autoFilter ref="A1:AH2" xr:uid="{A6B8DD7C-AAB7-4857-88E6-CB63ACE6C9CD}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{F4A78338-6595-4577-9E03-C526DD403CE7}" name="cpu_ticks"/>
     <tableColumn id="2" xr3:uid="{3FEDDFAD-B68B-49C8-A356-D67F960C915A}" name="ms_ticks"/>
     <tableColumn id="3" xr3:uid="{3A04F2C3-1866-458F-88A0-D09661ED4DF4}" name="cpu_count"/>
@@ -1363,7 +1323,7 @@
     <tableColumn id="16" xr3:uid="{E1A234A1-E64F-46B7-B885-8606FEE8A597}" name="scheduler_total_count"/>
     <tableColumn id="17" xr3:uid="{FEBFF05F-A9CF-4223-9792-0ADA879F81A6}" name="deadlock_monitor_serial_number"/>
     <tableColumn id="18" xr3:uid="{793249C1-FF6B-4CE4-996B-76BCA312D801}" name="sqlserver_start_time_ms_ticks"/>
-    <tableColumn id="19" xr3:uid="{06292E30-63F3-4020-B8C5-BAA3E876F63C}" name="sqlserver_start_time" dataDxfId="0"/>
+    <tableColumn id="19" xr3:uid="{06292E30-63F3-4020-B8C5-BAA3E876F63C}" name="sqlserver_start_time" dataDxfId="10"/>
     <tableColumn id="20" xr3:uid="{E04BAAE3-3FC6-4B59-9C98-426E92F97D81}" name="affinity_type"/>
     <tableColumn id="21" xr3:uid="{F629596F-A9F2-4FB4-83C0-37312548DF18}" name="affinity_type_desc"/>
     <tableColumn id="22" xr3:uid="{8513385E-8766-4E2B-B489-07868FCA0057}" name="process_kernel_time_ms"/>
@@ -1374,23 +1334,20 @@
     <tableColumn id="27" xr3:uid="{84867091-CA7D-48D1-A5BB-6F5EBEE21E48}" name="virtual_machine_type_desc"/>
     <tableColumn id="28" xr3:uid="{7CE75959-BA07-4BBE-9613-27F470E23562}" name="softnuma_configuration"/>
     <tableColumn id="29" xr3:uid="{27CCA778-281E-4309-81B2-97C8716C7704}" name="softnuma_configuration_desc"/>
-    <tableColumn id="30" xr3:uid="{8F313D84-C85C-40CC-92D2-29F89DCD5EAB}" name="process_physical_affinity"/>
     <tableColumn id="31" xr3:uid="{77CEBB32-6E6D-464C-9243-474BCAE49576}" name="sql_memory_model"/>
     <tableColumn id="32" xr3:uid="{AB42FC38-5227-4FD2-979A-C9178BB343CE}" name="sql_memory_model_desc"/>
     <tableColumn id="33" xr3:uid="{B87DB05E-FFA4-4108-9C04-A19FCAC32653}" name="socket_count"/>
     <tableColumn id="34" xr3:uid="{AC8E3438-8FAB-494C-B9DB-9C0D0FB8640C}" name="cores_per_socket"/>
     <tableColumn id="35" xr3:uid="{3CA7A67B-30FB-4230-BB84-42621FB0307C}" name="numa_node_count"/>
-    <tableColumn id="36" xr3:uid="{4656A1C9-8383-4C01-AAAE-1DC7E0A37BD5}" name="container_type"/>
-    <tableColumn id="37" xr3:uid="{E8992132-6F5D-46A6-86EF-7BD5A2D270B2}" name="container_type_desc"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4CAADD08-DBD5-4AD2-AA6D-225DF1B2ECAD}" name="Table12" displayName="Table12" ref="A1:O2" totalsRowShown="0">
-  <autoFilter ref="A1:O2" xr:uid="{4CAADD08-DBD5-4AD2-AA6D-225DF1B2ECAD}"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4CAADD08-DBD5-4AD2-AA6D-225DF1B2ECAD}" name="Table12" displayName="Table12" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{4CAADD08-DBD5-4AD2-AA6D-225DF1B2ECAD}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{6E473149-19C0-436C-8B91-E0CB14D5D85A}" name="database_id"/>
     <tableColumn id="2" xr3:uid="{C3F39C73-2BEF-4133-A5E5-4F3331615C93}" name="schema_id"/>
     <tableColumn id="3" xr3:uid="{EA331711-5149-44DE-94F0-775DD5D4F7F4}" name="schema_name"/>
@@ -1398,8 +1355,6 @@
     <tableColumn id="5" xr3:uid="{75EBD45A-DE6E-4EEE-9057-222B897778AB}" name="object_name"/>
     <tableColumn id="6" xr3:uid="{DCC125DF-2CF9-4CCD-80BA-79340DFD03EB}" name="stats_id"/>
     <tableColumn id="7" xr3:uid="{422D4DAD-AAE1-4965-93D3-668C2C3F4194}" name="stats_name"/>
-    <tableColumn id="8" xr3:uid="{531D3C09-0E1D-4A20-9531-B5DE31B7DEDB}" name="object_id2"/>
-    <tableColumn id="9" xr3:uid="{32EF27CD-FEF3-44D3-9E6C-8F0DDA9B18AB}" name="stats_id3"/>
     <tableColumn id="10" xr3:uid="{AD045917-C0F2-448A-864A-2BAC511D7272}" name="step_number"/>
     <tableColumn id="11" xr3:uid="{82EA9806-67FD-4B85-9962-F06DD850D09D}" name="range_high_key"/>
     <tableColumn id="12" xr3:uid="{BA9E706F-0AB9-4AF1-95CE-92A4F9FCBB4D}" name="range_rows"/>
@@ -1418,7 +1373,7 @@
     <tableColumn id="1" xr3:uid="{2371C3FF-E1D8-4768-9EB7-0FA51A478EDC}" name="ServerName_s"/>
     <tableColumn id="2" xr3:uid="{7BBA6DC6-36D1-4D30-ADD6-C02E2043FE09}" name="record_id_d"/>
     <tableColumn id="3" xr3:uid="{5FF6B684-4C9B-438D-80AE-420FEDAD3C39}" name="timestamp_d"/>
-    <tableColumn id="4" xr3:uid="{2F0ED155-E681-4A37-8A88-B65DEE436BD4}" name="timestamp_datetime" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{2F0ED155-E681-4A37-8A88-B65DEE436BD4}" name="timestamp_datetime" dataDxfId="9"/>
     <tableColumn id="5" xr3:uid="{3463BDB4-332F-4798-B2CE-F1047A46AD4C}" name="sql_cpu_d"/>
     <tableColumn id="6" xr3:uid="{13C5E21B-F3D0-48CD-AAEE-22E17DBF17A3}" name="idle_cpu_d"/>
     <tableColumn id="7" xr3:uid="{5EA7BA56-5ED4-4BE5-944F-C0922BC64496}" name="other_cpu_d"/>
@@ -1543,27 +1498,27 @@
     <tableColumn id="5" xr3:uid="{E3C50696-2DF6-484B-9CC5-F6A63497E94B}" name="user_scans"/>
     <tableColumn id="6" xr3:uid="{386BD38C-0AE9-47FC-9B4D-9F4D394ABD8B}" name="user_lookups"/>
     <tableColumn id="7" xr3:uid="{01B932C8-92B8-4277-B3D9-A9AE39577056}" name="user_updates"/>
-    <tableColumn id="8" xr3:uid="{C3E5BE79-FFEF-4B16-9789-5C0044EADC84}" name="last_user_seek" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{11C49885-2A3C-4462-89E4-664D1A59C4B7}" name="last_user_scan" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{E5E4B8AD-F430-49D1-B65A-421E0A7CFDF7}" name="last_user_lookup" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{DC039DE2-C9B9-40BB-B4D5-05EE8C9040B3}" name="last_user_update" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{C3E5BE79-FFEF-4B16-9789-5C0044EADC84}" name="last_user_seek" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{11C49885-2A3C-4462-89E4-664D1A59C4B7}" name="last_user_scan" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{E5E4B8AD-F430-49D1-B65A-421E0A7CFDF7}" name="last_user_lookup" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{DC039DE2-C9B9-40BB-B4D5-05EE8C9040B3}" name="last_user_update" dataDxfId="5"/>
     <tableColumn id="12" xr3:uid="{A073FE55-50AC-4479-8C3B-7B25AA30CCAC}" name="system_seeks"/>
     <tableColumn id="13" xr3:uid="{0F6309D4-0D6E-4AD6-AEAE-2A274B502951}" name="system_scans"/>
     <tableColumn id="14" xr3:uid="{DCC3CE1E-11F9-4A50-88F7-FCD8E280010E}" name="system_lookups"/>
     <tableColumn id="15" xr3:uid="{BD0A8475-696B-44D2-81AA-79B5C350A586}" name="system_updates"/>
-    <tableColumn id="16" xr3:uid="{DA729497-0017-44D4-A880-36A2A1972E39}" name="last_system_seek" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{172DA864-2310-4B69-BF7D-E8D9F325F765}" name="last_system_scan" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{019F50A5-DDEA-423E-AAF2-3650EA866E9B}" name="last_system_lookup" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{1D34997E-47AB-4B29-9B50-242BC31D929F}" name="last_system_update" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{DA729497-0017-44D4-A880-36A2A1972E39}" name="last_system_seek" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{172DA864-2310-4B69-BF7D-E8D9F325F765}" name="last_system_scan" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{019F50A5-DDEA-423E-AAF2-3650EA866E9B}" name="last_system_lookup" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{1D34997E-47AB-4B29-9B50-242BC31D929F}" name="last_system_update" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{69BE8402-C351-4A29-B6A8-3D80780FFA15}" name="Table10" displayName="Table10" ref="A1:AY2" totalsRowShown="0">
-  <autoFilter ref="A1:AY2" xr:uid="{69BE8402-C351-4A29-B6A8-3D80780FFA15}"/>
-  <tableColumns count="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{69BE8402-C351-4A29-B6A8-3D80780FFA15}" name="Table10" displayName="Table10" ref="A1:AS2" totalsRowShown="0">
+  <autoFilter ref="A1:AS2" xr:uid="{69BE8402-C351-4A29-B6A8-3D80780FFA15}"/>
+  <tableColumns count="45">
     <tableColumn id="1" xr3:uid="{1448FE5A-95F3-43A3-B1B6-1AECC8ECE67C}" name="database_id"/>
     <tableColumn id="2" xr3:uid="{FD383874-B726-4B15-AD8E-7C980BC80852}" name="object_id"/>
     <tableColumn id="3" xr3:uid="{4DD7E312-310A-44D1-B4B0-D938BB63C86E}" name="index_id"/>
@@ -1609,21 +1564,15 @@
     <tableColumn id="43" xr3:uid="{F9DC1F7E-3A24-42B4-9AD6-30E7B5612151}" name="tree_page_io_latch_wait_in_ms"/>
     <tableColumn id="44" xr3:uid="{38FD370C-B8EA-4717-A532-7D97CC31C695}" name="page_compression_attempt_count"/>
     <tableColumn id="45" xr3:uid="{24F00161-F5D5-4227-843C-E2CA19AC3D76}" name="page_compression_success_count"/>
-    <tableColumn id="46" xr3:uid="{3B3DDD0B-AA60-4045-9346-2DB2AB7378F1}" name="version_generated_inrow"/>
-    <tableColumn id="47" xr3:uid="{A1A008D8-8955-4E73-8150-D9C5A30FB61B}" name="version_generated_offrow"/>
-    <tableColumn id="48" xr3:uid="{1C6BD580-641A-4F03-8C8D-6FE8D45D67D4}" name="ghost_version_inrow"/>
-    <tableColumn id="49" xr3:uid="{992BF800-A756-472E-ACEA-9E9008FFF5B9}" name="ghost_version_offrow"/>
-    <tableColumn id="50" xr3:uid="{183BFCC9-5BF8-42EF-A718-976F2C7A2ED5}" name="insert_over_ghost_version_inrow"/>
-    <tableColumn id="51" xr3:uid="{D2D753DF-F35C-443C-996B-10A78CC12875}" name="insert_over_ghost_version_offrow"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}" name="Table11" displayName="Table11" ref="A1:X2" totalsRowShown="0">
-  <autoFilter ref="A1:X2" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}" name="Table11" displayName="Table11" ref="A1:V2" totalsRowShown="0">
+  <autoFilter ref="A1:V2" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{61888DB5-7723-4C9A-8D5B-C81CCB6ED9E6}" name="database_id"/>
     <tableColumn id="2" xr3:uid="{A86720A0-06D0-40AD-9F6B-1B855952AC6C}" name="schema_id"/>
     <tableColumn id="3" xr3:uid="{8F0A9D85-CC5A-4861-A2F3-DDC6CC8CD54C}" name="schema_name"/>
@@ -1638,10 +1587,8 @@
     <tableColumn id="12" xr3:uid="{78D5D7D1-96F0-4CDD-B2A1-E527CCB483AF}" name="filter_definition"/>
     <tableColumn id="13" xr3:uid="{1ABA3DBF-5D2A-4BBB-98FF-33849B90EB35}" name="is_temporary"/>
     <tableColumn id="14" xr3:uid="{96E6B6B8-1B2C-4A9D-B210-1AFE5A179C0A}" name="is_incremental"/>
-    <tableColumn id="15" xr3:uid="{44D05229-D118-4029-AA05-EAC02B449F6C}" name="has_persisted_sample"/>
-    <tableColumn id="16" xr3:uid="{ED760D8E-E7A2-4396-B909-D4D171C5C39E}" name="stats_generation_method_desc"/>
     <tableColumn id="17" xr3:uid="{38EF12FA-51C5-4EE8-88DD-2B03C7A2C1E6}" name="stats_columns"/>
-    <tableColumn id="18" xr3:uid="{55E4D7C1-B7C8-44B5-AEB9-B5295B0A1B42}" name="last_updated" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{55E4D7C1-B7C8-44B5-AEB9-B5295B0A1B42}" name="last_updated" dataDxfId="0"/>
     <tableColumn id="19" xr3:uid="{E1068D45-CB37-405C-B69F-3FF11CD0BADF}" name="rows"/>
     <tableColumn id="20" xr3:uid="{7E666E1D-950B-4E36-BBF2-9EF8063C1503}" name="rows_sampled"/>
     <tableColumn id="21" xr3:uid="{59FBFE22-CD62-4975-A9B1-C9A117EB6357}" name="steps"/>
@@ -1970,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0661C765-C8E7-4DC8-AF6F-DB3B4AE217B2}">
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1996,7 +1943,7 @@
     <col min="16" max="16" width="20.86328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29.86328125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.3984375" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="22.9296875" bestFit="1" customWidth="1"/>
@@ -2007,17 +1954,14 @@
     <col min="27" max="27" width="24.73046875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21.9296875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.19921875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -2031,19 +1975,19 @@
         <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="F1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="G1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="H1" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="I1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="J1" t="s">
         <v>53</v>
@@ -2072,7 +2016,7 @@
       <c r="R1" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>62</v>
       </c>
       <c r="T1" t="s">
@@ -2119,15 +2063,6 @@
       </c>
       <c r="AH1" t="s">
         <v>77</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2140,7 +2075,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5216EEC-EE56-469C-B0AC-60F6560CE05C}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2160,19 +2095,17 @@
     <col min="12" max="12" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.9296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.3984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.53125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.06640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.53125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.06640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2189,61 +2122,55 @@
         <v>31</v>
       </c>
       <c r="F1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" t="s">
+        <v>161</v>
+      </c>
+      <c r="O1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G1" t="s">
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
         <v>164</v>
       </c>
-      <c r="H1" t="s">
+      <c r="S1" t="s">
         <v>165</v>
       </c>
-      <c r="I1" t="s">
+      <c r="T1" t="s">
         <v>166</v>
       </c>
-      <c r="J1" t="s">
+      <c r="U1" t="s">
         <v>167</v>
       </c>
-      <c r="K1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="V1" t="s">
         <v>168</v>
-      </c>
-      <c r="M1" t="s">
-        <v>169</v>
-      </c>
-      <c r="N1" t="s">
-        <v>170</v>
-      </c>
-      <c r="O1" t="s">
-        <v>171</v>
-      </c>
-      <c r="P1" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>173</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="S1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" t="s">
-        <v>175</v>
-      </c>
-      <c r="U1" t="s">
-        <v>176</v>
-      </c>
-      <c r="V1" t="s">
-        <v>177</v>
-      </c>
-      <c r="W1" t="s">
-        <v>178</v>
-      </c>
-      <c r="X1" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2256,7 +2183,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB8D599-8A21-4C49-8BBE-5F2B5EFE4765}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2270,16 +2197,14 @@
     <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.9296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.53125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.53125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2296,34 +2221,28 @@
         <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H1" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="I1" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="J1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="K1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="L1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="M1" t="s">
-        <v>183</v>
-      </c>
-      <c r="N1" t="s">
-        <v>184</v>
-      </c>
-      <c r="O1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2355,29 +2274,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D2" s="4"/>
+      <c r="D2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2406,19 +2325,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2599,17 +2518,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+        <v>175</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2775,25 +2690,25 @@
         <v>35</v>
       </c>
       <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>94</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>96</v>
-      </c>
-      <c r="M1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" t="s">
-        <v>98</v>
-      </c>
-      <c r="O1" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2820,18 +2735,18 @@
     <col min="5" max="5" width="11.3984375" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="13.1328125" customWidth="1"/>
-    <col min="8" max="8" width="14.06640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="14.19921875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="15.796875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="15.9296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.06640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.796875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.9296875" style="4" customWidth="1"/>
     <col min="12" max="12" width="13.46484375" customWidth="1"/>
     <col min="13" max="13" width="13.59765625" customWidth="1"/>
     <col min="14" max="14" width="15.19921875" customWidth="1"/>
     <col min="15" max="15" width="15.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16.265625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="16.3984375" style="5" customWidth="1"/>
-    <col min="18" max="18" width="18" style="5" customWidth="1"/>
-    <col min="19" max="19" width="18.1328125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="16.265625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="16.3984375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="18" style="4" customWidth="1"/>
+    <col min="19" max="19" width="18.1328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.45">
@@ -2845,52 +2760,52 @@
         <v>33</v>
       </c>
       <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" t="s">
         <v>107</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>108</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +2818,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E7ECA2-EE80-49B3-90E8-9B13C361D86F}">
-  <dimension ref="A1:AY1"/>
+  <dimension ref="A1:AS1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2956,15 +2871,9 @@
     <col min="43" max="43" width="27.73046875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="30.53125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="30.73046875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.1328125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.86328125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.06640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="29.19921875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="29.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2978,145 +2887,127 @@
         <v>37</v>
       </c>
       <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" t="s">
         <v>116</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>117</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>120</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>121</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>122</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>123</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>124</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>125</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>126</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>128</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>129</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>130</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>131</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>132</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>133</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>134</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>135</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>136</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>137</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>138</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>139</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>140</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>141</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>142</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>143</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>144</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>145</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>146</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>147</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>148</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>149</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>150</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>151</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>152</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>153</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>157</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>158</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>160</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>161</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>